<commit_message>
updating environmental data extraction
Former-commit-id: ae3a514582944b249a18351426f5ac96ad129881
</commit_message>
<xml_diff>
--- a/Data/acc_data_reformatted_sorted.xlsx
+++ b/Data/acc_data_reformatted_sorted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joribarley/Documents/GitHub/plasticity/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77D1907-122A-A948-AEC4-0BF05F17DFBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C43E6E-7779-E14C-8D9E-745DD651B7EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{71CED034-CA02-F342-B8AB-E8372AC16A5C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{71CED034-CA02-F342-B8AB-E8372AC16A5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1916,10 +1916,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD823B55-7788-6E47-847E-5FF5E4B6C294}">
   <dimension ref="A1:AL603"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A542" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="R569" sqref="R569"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -62442,7 +62442,7 @@
         <v>387</v>
       </c>
       <c r="Q529" s="15">
-        <v>33.67</v>
+        <v>-33.67</v>
       </c>
       <c r="R529">
         <v>19.62</v>
@@ -62540,7 +62540,7 @@
         <v>387</v>
       </c>
       <c r="Q530" s="16">
-        <v>33.67</v>
+        <v>-33.67</v>
       </c>
       <c r="R530" s="2">
         <v>19.62</v>
@@ -62638,7 +62638,7 @@
         <v>387</v>
       </c>
       <c r="Q531" s="16">
-        <v>33.67</v>
+        <v>-33.67</v>
       </c>
       <c r="R531" s="2">
         <v>19.62</v>
@@ -62736,7 +62736,7 @@
         <v>390</v>
       </c>
       <c r="Q532" s="37">
-        <v>33.39</v>
+        <v>-33.39</v>
       </c>
       <c r="R532">
         <v>18.57</v>
@@ -62834,7 +62834,7 @@
         <v>390</v>
       </c>
       <c r="Q533" s="38">
-        <v>33.39</v>
+        <v>-33.39</v>
       </c>
       <c r="R533" s="2">
         <v>18.57</v>
@@ -62932,7 +62932,7 @@
         <v>390</v>
       </c>
       <c r="Q534" s="38">
-        <v>33.39</v>
+        <v>-33.39</v>
       </c>
       <c r="R534" s="2">
         <v>18.57</v>
@@ -63030,7 +63030,7 @@
         <v>391</v>
       </c>
       <c r="Q535" s="15">
-        <v>33.01</v>
+        <v>-33.01</v>
       </c>
       <c r="R535">
         <v>19</v>
@@ -63128,7 +63128,7 @@
         <v>391</v>
       </c>
       <c r="Q536" s="15">
-        <v>33.01</v>
+        <v>-33.01</v>
       </c>
       <c r="R536">
         <v>19</v>
@@ -63226,7 +63226,7 @@
         <v>391</v>
       </c>
       <c r="Q537" s="15">
-        <v>33.01</v>
+        <v>-33.01</v>
       </c>
       <c r="R537">
         <v>19</v>
@@ -63325,7 +63325,7 @@
         <v>392</v>
       </c>
       <c r="Q538" s="15">
-        <v>33.340000000000003</v>
+        <v>-33.340000000000003</v>
       </c>
       <c r="R538">
         <v>19.57</v>
@@ -63428,7 +63428,7 @@
         <v>392</v>
       </c>
       <c r="Q539" s="15">
-        <v>33.340000000000003</v>
+        <v>-33.340000000000003</v>
       </c>
       <c r="R539">
         <v>19.57</v>
@@ -63526,7 +63526,7 @@
         <v>392</v>
       </c>
       <c r="Q540" s="15">
-        <v>33.340000000000003</v>
+        <v>-33.340000000000003</v>
       </c>
       <c r="R540">
         <v>19.57</v>
@@ -63624,7 +63624,7 @@
         <v>393</v>
       </c>
       <c r="Q541" s="15">
-        <v>25.06</v>
+        <v>-25.06</v>
       </c>
       <c r="R541">
         <v>31.05</v>
@@ -63722,7 +63722,7 @@
         <v>393</v>
       </c>
       <c r="Q542" s="15">
-        <v>25.06</v>
+        <v>-25.06</v>
       </c>
       <c r="R542">
         <v>31.05</v>
@@ -63820,7 +63820,7 @@
         <v>393</v>
       </c>
       <c r="Q543" s="15">
-        <v>25.06</v>
+        <v>-25.06</v>
       </c>
       <c r="R543">
         <v>31.05</v>
@@ -63918,7 +63918,7 @@
         <v>394</v>
       </c>
       <c r="Q544" s="15">
-        <v>28.47</v>
+        <v>-28.47</v>
       </c>
       <c r="R544">
         <v>20.46</v>
@@ -64016,7 +64016,7 @@
         <v>394</v>
       </c>
       <c r="Q545" s="15">
-        <v>28.47</v>
+        <v>-28.47</v>
       </c>
       <c r="R545">
         <v>20.46</v>
@@ -64114,7 +64114,7 @@
         <v>394</v>
       </c>
       <c r="Q546" s="15">
-        <v>28.47</v>
+        <v>-28.47</v>
       </c>
       <c r="R546">
         <v>20.46</v>
@@ -64212,7 +64212,7 @@
         <v>395</v>
       </c>
       <c r="Q547" s="17">
-        <v>23.05</v>
+        <v>-23.05</v>
       </c>
       <c r="R547">
         <v>30.17</v>
@@ -64310,7 +64310,7 @@
         <v>395</v>
       </c>
       <c r="Q548" s="17">
-        <v>23.05</v>
+        <v>-23.05</v>
       </c>
       <c r="R548">
         <v>30.17</v>
@@ -64408,7 +64408,7 @@
         <v>395</v>
       </c>
       <c r="Q549" s="17">
-        <v>23.05</v>
+        <v>-23.05</v>
       </c>
       <c r="R549">
         <v>30.17</v>
@@ -64506,7 +64506,7 @@
         <v>396</v>
       </c>
       <c r="Q550">
-        <v>1.28</v>
+        <v>-1.28</v>
       </c>
       <c r="R550">
         <v>36.82</v>
@@ -64604,7 +64604,7 @@
         <v>396</v>
       </c>
       <c r="Q551">
-        <v>1.28</v>
+        <v>-1.28</v>
       </c>
       <c r="R551">
         <v>36.82</v>
@@ -64702,7 +64702,7 @@
         <v>396</v>
       </c>
       <c r="Q552">
-        <v>1.28</v>
+        <v>-1.28</v>
       </c>
       <c r="R552">
         <v>36.82</v>
@@ -64800,7 +64800,7 @@
         <v>387</v>
       </c>
       <c r="Q553" s="15">
-        <v>33.67</v>
+        <v>-33.67</v>
       </c>
       <c r="R553">
         <v>19.62</v>
@@ -64898,7 +64898,7 @@
         <v>387</v>
       </c>
       <c r="Q554" s="16">
-        <v>33.67</v>
+        <v>-33.67</v>
       </c>
       <c r="R554" s="2">
         <v>19.62</v>
@@ -64996,7 +64996,7 @@
         <v>387</v>
       </c>
       <c r="Q555" s="16">
-        <v>33.67</v>
+        <v>-33.67</v>
       </c>
       <c r="R555" s="2">
         <v>19.62</v>
@@ -65094,7 +65094,7 @@
         <v>390</v>
       </c>
       <c r="Q556" s="37">
-        <v>33.39</v>
+        <v>-33.39</v>
       </c>
       <c r="R556">
         <v>18.57</v>
@@ -65192,7 +65192,7 @@
         <v>390</v>
       </c>
       <c r="Q557" s="38">
-        <v>33.39</v>
+        <v>-33.39</v>
       </c>
       <c r="R557" s="2">
         <v>18.57</v>
@@ -65290,7 +65290,7 @@
         <v>390</v>
       </c>
       <c r="Q558" s="38">
-        <v>33.39</v>
+        <v>-33.39</v>
       </c>
       <c r="R558" s="2">
         <v>18.57</v>
@@ -65388,7 +65388,7 @@
         <v>391</v>
       </c>
       <c r="Q559" s="15">
-        <v>33.01</v>
+        <v>-33.01</v>
       </c>
       <c r="R559">
         <v>19</v>
@@ -65486,7 +65486,7 @@
         <v>391</v>
       </c>
       <c r="Q560" s="15">
-        <v>33.01</v>
+        <v>-33.01</v>
       </c>
       <c r="R560">
         <v>19</v>
@@ -65584,7 +65584,7 @@
         <v>391</v>
       </c>
       <c r="Q561" s="15">
-        <v>33.01</v>
+        <v>-33.01</v>
       </c>
       <c r="R561">
         <v>19</v>
@@ -65682,7 +65682,7 @@
         <v>392</v>
       </c>
       <c r="Q562" s="15">
-        <v>33.340000000000003</v>
+        <v>-33.340000000000003</v>
       </c>
       <c r="R562">
         <v>19.57</v>
@@ -65780,7 +65780,7 @@
         <v>392</v>
       </c>
       <c r="Q563" s="15">
-        <v>33.340000000000003</v>
+        <v>-33.340000000000003</v>
       </c>
       <c r="R563">
         <v>19.57</v>
@@ -65878,7 +65878,7 @@
         <v>392</v>
       </c>
       <c r="Q564" s="15">
-        <v>33.340000000000003</v>
+        <v>-33.340000000000003</v>
       </c>
       <c r="R564">
         <v>19.57</v>
@@ -65976,7 +65976,7 @@
         <v>393</v>
       </c>
       <c r="Q565" s="15">
-        <v>25.06</v>
+        <v>-25.06</v>
       </c>
       <c r="R565">
         <v>31.05</v>
@@ -66074,7 +66074,7 @@
         <v>393</v>
       </c>
       <c r="Q566" s="15">
-        <v>25.06</v>
+        <v>-25.06</v>
       </c>
       <c r="R566">
         <v>31.05</v>
@@ -66172,7 +66172,7 @@
         <v>393</v>
       </c>
       <c r="Q567" s="15">
-        <v>25.06</v>
+        <v>-25.06</v>
       </c>
       <c r="R567">
         <v>31.05</v>
@@ -66270,7 +66270,7 @@
         <v>394</v>
       </c>
       <c r="Q568" s="15">
-        <v>28.47</v>
+        <v>-28.47</v>
       </c>
       <c r="R568">
         <v>20.46</v>
@@ -66368,7 +66368,7 @@
         <v>394</v>
       </c>
       <c r="Q569" s="15">
-        <v>28.47</v>
+        <v>-28.47</v>
       </c>
       <c r="R569">
         <v>20.46</v>
@@ -66466,7 +66466,7 @@
         <v>394</v>
       </c>
       <c r="Q570" s="15">
-        <v>28.47</v>
+        <v>-28.47</v>
       </c>
       <c r="R570">
         <v>20.46</v>
@@ -66564,7 +66564,7 @@
         <v>395</v>
       </c>
       <c r="Q571" s="17">
-        <v>23.05</v>
+        <v>-23.05</v>
       </c>
       <c r="R571">
         <v>30.17</v>
@@ -66662,7 +66662,7 @@
         <v>395</v>
       </c>
       <c r="Q572" s="17">
-        <v>23.05</v>
+        <v>-23.05</v>
       </c>
       <c r="R572">
         <v>30.17</v>
@@ -66760,7 +66760,7 @@
         <v>395</v>
       </c>
       <c r="Q573" s="17">
-        <v>23.05</v>
+        <v>-23.05</v>
       </c>
       <c r="R573">
         <v>30.17</v>
@@ -66858,8 +66858,8 @@
       <c r="P574" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="Q574" s="3">
-        <v>1.28</v>
+      <c r="Q574">
+        <v>-1.28</v>
       </c>
       <c r="R574" s="3">
         <v>36.82</v>
@@ -66957,8 +66957,8 @@
       <c r="P575" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="Q575" s="3">
-        <v>1.28</v>
+      <c r="Q575">
+        <v>-1.28</v>
       </c>
       <c r="R575" s="3">
         <v>36.82</v>
@@ -67056,8 +67056,8 @@
       <c r="P576" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="Q576" s="3">
-        <v>1.28</v>
+      <c r="Q576">
+        <v>-1.28</v>
       </c>
       <c r="R576" s="3">
         <v>36.82</v>

</xml_diff>